<commit_message>
แก้ export excel WH
</commit_message>
<xml_diff>
--- a/local/public/excel_files/consignments.xlsx
+++ b/local/public/excel_files/consignments.xlsx
@@ -74,19 +74,19 @@
     <t>Service Code (รหัสบริการ)</t>
   </si>
   <si>
+    <t>P100003</t>
+  </si>
+  <si>
+    <t>คุณ ศิลปการสกุล  ภัทร์พงศกร</t>
+  </si>
+  <si>
+    <t>(ตย.)2102/1 อาคารไอยเรศวร 4 ซ.ลาดพร้าว84 สู่ความสำเร็จ , ต.แขวงวังทองหลาง , อ.เขตวังทองหลาง, จ.กรุงเทพมหานคร</t>
+  </si>
+  <si>
     <t>P100004</t>
   </si>
   <si>
-    <t>คุณ อธิษฐ์โภคิน  ภัทร์รัฐชัย</t>
-  </si>
-  <si>
-    <t>(ตย.)2102/1 อาคารไอยเรศวร 4 ซ.ลาดพร้าว84 สู่ความสำเร็จ , ต.แขวงวังทองหลาง , อ.เขตวังทองหลาง, จ.กรุงเทพมหานคร</t>
-  </si>
-  <si>
-    <t>O122011800006</t>
-  </si>
-  <si>
-    <t>คุณ ปริยากรโสภณ  พงศ์บุณยภา</t>
+    <t>111 หมู่บ้าน qqqqq , ต.บ้านระกาศ , อ.บางบ่อ, จ.สมุทรปราการ</t>
   </si>
 </sst>
 </file>
@@ -437,7 +437,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:S9"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1:S1"/>
@@ -592,13 +592,13 @@
       <c r="B4"/>
       <c r="C4"/>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G4">
         <v>10560</v>
@@ -618,129 +618,36 @@
       <c r="R4"/>
       <c r="S4"/>
     </row>
-    <row r="6" spans="1:19">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6" t="s">
+    <row r="5" spans="1:19">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
         <v>23</v>
       </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6">
+      <c r="G5">
         <v>10560</v>
       </c>
-      <c r="H6"/>
-      <c r="I6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6"/>
-      <c r="L6"/>
-      <c r="M6"/>
-      <c r="N6"/>
-      <c r="O6"/>
-      <c r="P6"/>
-      <c r="Q6"/>
-      <c r="R6"/>
-      <c r="S6"/>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7">
-        <v>10560</v>
-      </c>
-      <c r="H7"/>
-      <c r="I7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7"/>
-      <c r="K7"/>
-      <c r="L7"/>
-      <c r="M7"/>
-      <c r="N7"/>
-      <c r="O7"/>
-      <c r="P7"/>
-      <c r="Q7"/>
-      <c r="R7"/>
-      <c r="S7"/>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8">
-        <v>10560</v>
-      </c>
-      <c r="H8"/>
-      <c r="I8" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8"/>
-      <c r="K8"/>
-      <c r="L8"/>
-      <c r="M8"/>
-      <c r="N8"/>
-      <c r="O8"/>
-      <c r="P8"/>
-      <c r="Q8"/>
-      <c r="R8"/>
-      <c r="S8"/>
-    </row>
-    <row r="9" spans="1:19">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9">
-        <v>10560</v>
-      </c>
-      <c r="H9"/>
-      <c r="I9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J9"/>
-      <c r="K9"/>
-      <c r="L9"/>
-      <c r="M9"/>
-      <c r="N9"/>
-      <c r="O9"/>
-      <c r="P9"/>
-      <c r="Q9"/>
-      <c r="R9"/>
-      <c r="S9"/>
+      <c r="H5"/>
+      <c r="I5" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>